<commit_message>
quote puller done, now working on shuffle
</commit_message>
<xml_diff>
--- a/quotes.xlsx
+++ b/quotes.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katt/Code/twitterbot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D5961BAC-F7D6-AE4C-9927-E296B393AB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2363294F-D2D9-5741-A8C1-AEB159400655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="9580" yWindow="6660" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quotes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,166 +42,166 @@
     <t>Epictetus</t>
   </si>
   <si>
-    <t>Don't explain your philosophy. Embody it.</t>
-  </si>
-  <si>
-    <t>There is only one way to happiness and that is to cease worrying about things which are beyond the power or our will.</t>
-  </si>
-  <si>
-    <t>First say to yourself what you would be; and then do what you have to do.</t>
-  </si>
-  <si>
-    <t>It is impossible for a man to learn what he thinks he already knows.</t>
-  </si>
-  <si>
-    <t>Only the educated are free.</t>
-  </si>
-  <si>
-    <t>You are a little soul carrying around a corpse</t>
-  </si>
-  <si>
-    <t>No man is free who is not master of himself.</t>
-  </si>
-  <si>
-    <t>Do not try to seem wise to others.</t>
-  </si>
-  <si>
-    <t>No great thing is created suddenly.</t>
-  </si>
-  <si>
     <t>Marcus Aurelius</t>
   </si>
   <si>
-    <t>The happiness of your life depends upon the quality of your thoughts.</t>
-  </si>
-  <si>
-    <t>Waste no more time arguing about what a good man should be. Be one.</t>
-  </si>
-  <si>
-    <t>The best revenge is to be unlike him who performed the injury.</t>
-  </si>
-  <si>
-    <t>The soul becomes dyed with the colour of its thoughts.</t>
-  </si>
-  <si>
-    <t>How much more grievous are the consequences of anger than the causes of it.</t>
-  </si>
-  <si>
-    <t>The first rule is to keep an untroubled spirit. The second is to look things in the face and know them for what they are.</t>
-  </si>
-  <si>
-    <t>Look well into thyself; there is a source of strength which will always spring up if thou wilt always look.</t>
-  </si>
-  <si>
-    <t>You always own the option of having no opinion. There is never any need to get worked up or to trouble your soul about things you can't control. These things are not asking to be judged by you. Leave them alone.</t>
-  </si>
-  <si>
-    <t>What we do now echoes in eternity.</t>
-  </si>
-  <si>
-    <t>Never esteem anything as of advantage to you that will make you break your word or lose your self-respect.</t>
-  </si>
-  <si>
-    <t>Your days are numbered. Use them to throw open the windows of your soul to the sun. If you do not</t>
-  </si>
-  <si>
-    <t>Just that you do the right thing. The rest doesn't matter. Cold or warm. Tired or well-rested. Despised or honored.</t>
-  </si>
-  <si>
-    <t>Nowhere can man find a quieter or more untroubled retreat than in his own soul.</t>
-  </si>
-  <si>
-    <t>Be like the cliff against which the waves continually break; but it stands firm and tames the fury of the water around it.</t>
-  </si>
-  <si>
-    <t>Death smiles at us all; all we can do is smile back.</t>
-  </si>
-  <si>
     <t>Cicero</t>
   </si>
   <si>
-    <t>Knowledge which is divorced from justice may be called cunning rather than wisdom.</t>
-  </si>
-  <si>
-    <t>To be content with what we possess is the greatest and most secure of riches.</t>
-  </si>
-  <si>
-    <t>It is the peculiar quality of a fool to perceive the faults of others and to forget his own.</t>
-  </si>
-  <si>
-    <t>Cultivation of the mind is as necessary as food to the body</t>
-  </si>
-  <si>
-    <t>Wealth consists not in having great possessions, but in having few wants.</t>
-  </si>
-  <si>
-    <t>If you want to improve, be content to be thought foolish and stupid.</t>
-  </si>
-  <si>
-    <t>Circumstances don't make the man, they only reveal him to himself.</t>
-  </si>
-  <si>
-    <t>The greater the difficulty, the more glory in surmounting it. Skillful pilots gain their reputation from storms and tempests.</t>
-  </si>
-  <si>
-    <t>A mind without instruction can no more bear fruit than can a field, however fertile, without cultivation.</t>
-  </si>
-  <si>
-    <t>Nobody can give you wiser advice than yourself: if you heed yourself, you'll never go wrong.</t>
-  </si>
-  <si>
-    <t>Our span of life is brief, but is long enough for us to live well and honestly.</t>
-  </si>
-  <si>
-    <t>It is foolish to tear one’s hair in grief, as though sorrow would be made less by baldness.</t>
-  </si>
-  <si>
-    <t>It is not by muscle, speed, or physical dexterity that great things are achieved, but by reflection, force of character, and judgment.</t>
-  </si>
-  <si>
-    <t>Friendship improves happiness, and abates misery, by doubling our joys, and dividing our grief.</t>
-  </si>
-  <si>
-    <t>The art of living is more like wrestling than dancing, in so far as it stands ready against the accidental and the unforeseen, and is not apt to fall.</t>
-  </si>
-  <si>
-    <t>Observe always that everything is the result of change, and get used to thinking that there is nothing Nature loves so well as to change existing forms and make new ones like them.</t>
-  </si>
-  <si>
-    <t>If any man despises me, that is his problem. My only concern is not doing or saying anything deserving of contempt.</t>
-  </si>
-  <si>
-    <t>Begin each day by telling yourself: Today I shall be meeting with interference, ingratitude, insolence, disloyalty, ill-will, and selfishness – all of them due to the offenders’ ignorance of what is good or evil.</t>
-  </si>
-  <si>
-    <t>How much time he gains who does not look to see what his neighbour says or does or thinks, but only at what he does himself, to make it just and holy.</t>
-  </si>
-  <si>
-    <t>Do not act as if you were going to live ten thousand years. Death hangs over you. While you live, while it is in your power, be good.</t>
-  </si>
-  <si>
-    <t>The object of life is not to be on the side of the majority, but to escape finding oneself in the ranks of the insane.</t>
-  </si>
-  <si>
-    <t>You have power over your mind - not outside events. Realize this, and you will find strength.</t>
-  </si>
-  <si>
-    <t>Know you not that a good man does nothing for appearance sake, but for the sake of having done right?</t>
-  </si>
-  <si>
-    <t>Preach not to others what they should eat, but eat as becomes you and be silent.</t>
-  </si>
-  <si>
-    <t>A ship should not ride on a single anchor, nor life on a single hope</t>
-  </si>
-  <si>
-    <t>Know, first, who you are, and then adorn yourself accordingly.</t>
+    <t>'Wealth consists not in having great possessions, but in having few wants.'</t>
+  </si>
+  <si>
+    <t>'Don't explain your philosophy. Embody it.'</t>
+  </si>
+  <si>
+    <t>'There is only one way to happiness and that is to cease worrying about things which are beyond the power or our will.'</t>
+  </si>
+  <si>
+    <t>'First say to yourself what you would be; and then do what you have to do.'</t>
+  </si>
+  <si>
+    <t>'If you want to improve, be content to be thought foolish and stupid.'</t>
+  </si>
+  <si>
+    <t>'It is impossible for a man to learn what he thinks he already knows.'</t>
+  </si>
+  <si>
+    <t>'Circumstances don't make the man, they only reveal him to himself.'</t>
+  </si>
+  <si>
+    <t>'Only the educated are free.'</t>
+  </si>
+  <si>
+    <t>'You are a little soul carrying around a corpse'</t>
+  </si>
+  <si>
+    <t>'No man is free who is not master of himself.'</t>
+  </si>
+  <si>
+    <t>'The greater the difficulty, the more glory in surmounting it. Skillful pilots gain their reputation from storms and tempests.'</t>
+  </si>
+  <si>
+    <t>'Do not try to seem wise to others.'</t>
+  </si>
+  <si>
+    <t>'Know, first, who you are, and then adorn yourself accordingly.'</t>
+  </si>
+  <si>
+    <t>'A ship should not ride on a single anchor, nor life on a single hope'</t>
+  </si>
+  <si>
+    <t>'Preach not to others what they should eat, but eat as becomes you and be silent.'</t>
+  </si>
+  <si>
+    <t>'Know you not that a good man does nothing for appearance sake, but for the sake of having done right?'</t>
+  </si>
+  <si>
+    <t>'No great thing is created suddenly.'</t>
+  </si>
+  <si>
+    <t>'You have power over your mind - not outside events. Realize this, and you will find strength.'</t>
+  </si>
+  <si>
+    <t>'The happiness of your life depends upon the quality of your thoughts.'</t>
+  </si>
+  <si>
+    <t>'Waste no more time arguing about what a good man should be. Be one.'</t>
+  </si>
+  <si>
+    <t>'The best revenge is to be unlike him who performed the injury.'</t>
+  </si>
+  <si>
+    <t>'The soul becomes dyed with the colour of its thoughts.'</t>
+  </si>
+  <si>
+    <t>'The object of life is not to be on the side of the majority, but to escape finding oneself in the ranks of the insane.'</t>
+  </si>
+  <si>
+    <t>'How much more grievous are the consequences of anger than the causes of it.'</t>
+  </si>
+  <si>
+    <t>'Do not act as if you were going to live ten thousand years. Death hangs over you. While you live, while it is in your power, be good.'</t>
+  </si>
+  <si>
+    <t>'The first rule is to keep an untroubled spirit. The second is to look things in the face and know them for what they are.'</t>
+  </si>
+  <si>
+    <t>'Look well into thyself; there is a source of strength which will always spring up if thou wilt always look.'</t>
+  </si>
+  <si>
+    <t>'How much time he gains who does not look to see what his neighbour says or does or thinks, but only at what he does himself, to make it just and holy.'</t>
+  </si>
+  <si>
+    <t>'Begin each day by telling yourself: Today I shall be meeting with interference, ingratitude, insolence, disloyalty, ill-will, and selfishness – all of them due to the offenders’ ignorance of what is good or evil.'</t>
+  </si>
+  <si>
+    <t>'You always own the option of having no opinion. There is never any need to get worked up or to trouble your soul about things you can't control. These things are not asking to be judged by you. Leave them alone.'</t>
+  </si>
+  <si>
+    <t>'What we do now echoes in eternity.'</t>
+  </si>
+  <si>
+    <t>'Never esteem anything as of advantage to you that will make you break your word or lose your self-respect.'</t>
+  </si>
+  <si>
+    <t>'Your days are numbered. Use them to throw open the windows of your soul to the sun. If you do not'</t>
+  </si>
+  <si>
+    <t>'Just that you do the right thing. The rest doesn't matter. Cold or warm. Tired or well-rested. Despised or honored.'</t>
+  </si>
+  <si>
+    <t>'If any man despises me, that is his problem. My only concern is not doing or saying anything deserving of contempt.'</t>
+  </si>
+  <si>
+    <t>'Observe always that everything is the result of change, and get used to thinking that there is nothing Nature loves so well as to change existing forms and make new ones like them.'</t>
+  </si>
+  <si>
+    <t>'Nowhere can man find a quieter or more untroubled retreat than in his own soul.'</t>
+  </si>
+  <si>
+    <t>'Be like the cliff against which the waves continually break; but it stands firm and tames the fury of the water around it.'</t>
+  </si>
+  <si>
+    <t>'The art of living is more like wrestling than dancing, in so far as it stands ready against the accidental and the unforeseen, and is not apt to fall.'</t>
+  </si>
+  <si>
+    <t>'Death smiles at us all; all we can do is smile back.'</t>
+  </si>
+  <si>
+    <t>'Friendship improves happiness, and abates misery, by doubling our joys, and dividing our grief.'</t>
+  </si>
+  <si>
+    <t>'It is not by muscle, speed, or physical dexterity that great things are achieved, but by reflection, force of character, and judgment.'</t>
+  </si>
+  <si>
+    <t>'It is foolish to tear one’s hair in grief, as though sorrow would be made less by baldness.'</t>
+  </si>
+  <si>
+    <t>'Our span of life is brief, but is long enough for us to live well and honestly.'</t>
+  </si>
+  <si>
+    <t>'Knowledge which is divorced from justice may be called cunning rather than wisdom.'</t>
+  </si>
+  <si>
+    <t>'Nobody can give you wiser advice than yourself: if you heed yourself, you'll never go wrong.'</t>
+  </si>
+  <si>
+    <t>'To be content with what we possess is the greatest and most secure of riches.'</t>
+  </si>
+  <si>
+    <t>'It is the peculiar quality of a fool to perceive the faults of others and to forget his own.'</t>
+  </si>
+  <si>
+    <t>'A mind without instruction can no more bear fruit than can a field, however fertile, without cultivation.'</t>
+  </si>
+  <si>
+    <t>'Cultivation of the mind is as necessary as food to the body'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1024,16 +1035,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B1:F1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="78" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1046,7 +1056,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -1054,7 +1064,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1062,7 +1072,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -1070,7 +1080,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -1078,7 +1088,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -1086,7 +1096,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -1094,7 +1104,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -1102,7 +1112,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -1110,7 +1120,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -1118,7 +1128,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -1126,7 +1136,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
@@ -1134,7 +1144,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -1142,7 +1152,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -1150,7 +1160,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -1158,7 +1168,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -1166,7 +1176,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
@@ -1174,7 +1184,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
@@ -1182,170 +1192,170 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1353,95 +1363,95 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>